<commit_message>
results imported to excel
</commit_message>
<xml_diff>
--- a/pythondata.xlsx
+++ b/pythondata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f72c30d29a410df/Masaüstü/finish_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="295" documentId="8_{025AF85D-C21F-4A00-BEF1-62C0000F1972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EA5AB72-C724-4AA1-BAF3-3C2FA11FD37C}"/>
+  <xr:revisionPtr revIDLastSave="296" documentId="8_{025AF85D-C21F-4A00-BEF1-62C0000F1972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E38E95EB-0279-4945-A990-D0B882017936}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4DDDD3FC-5805-4672-8E70-7CCE20338C5B}"/>
   </bookViews>
@@ -19,8 +19,8 @@
     <definedName name="Captable">sheetessah!$L$2:$M$31</definedName>
     <definedName name="Costabler">sheetessah!$A$34:$AD$63</definedName>
     <definedName name="ctable">sheetessah!$C$2:$C$7</definedName>
-    <definedName name="Demtable">sheetessah!$E$2:$J$31</definedName>
     <definedName name="ltable">sheetessah!$A$2:$A$31</definedName>
+    <definedName name="Suptable">sheetessah!$E$2:$J$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>